<commit_message>
write data in cell
</commit_message>
<xml_diff>
--- a/wcsm9seleniumproject/src/main/resources/TestData.xlsx
+++ b/wcsm9seleniumproject/src/main/resources/TestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Team</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">Captain</t>
   </si>
   <si>
+    <t xml:space="preserve">Location</t>
+  </si>
+  <si>
     <t xml:space="preserve">CSK</t>
   </si>
   <si>
@@ -86,6 +89,9 @@
   </si>
   <si>
     <t xml:space="preserve">SD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pune</t>
   </si>
 </sst>
 </file>
@@ -196,20 +202,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -230,10 +240,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="O6" activeCellId="0" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -245,85 +255,93 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>21</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>